<commit_message>
doing edits to make calculateDamLevel less shite
</commit_message>
<xml_diff>
--- a/Example_Data/Rebeccas_Excels/Reb_DailyFlowRates_Canmore.xlsx
+++ b/Example_Data/Rebeccas_Excels/Reb_DailyFlowRates_Canmore.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arebe\OneDrive\OneDocs\GitHub\C--Hacks2019\Example_Data\Rebeccas_Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{1DD41B2A-E8FD-4721-8707-3EDDB4E6CB23}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00BC6EAC-E5C8-40E0-8CE1-A101CA69A9A3}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="8_{1DD41B2A-E8FD-4721-8707-3EDDB4E6CB23}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{490BA540-E5F5-42F7-84D1-32F292E2F5C8}"/>
   <bookViews>
-    <workbookView xWindow="23595" yWindow="3735" windowWidth="10185" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18960" yWindow="4515" windowWidth="10185" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily__Feb-16-2019_09_00_16PM_D" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="29">
   <si>
     <t>﻿Daily Discharge (m3/s) (PARAM = 1)</t>
   </si>
@@ -106,6 +106,15 @@
   </si>
   <si>
     <t>Quartile</t>
+  </si>
+  <si>
+    <t>dec stdev</t>
+  </si>
+  <si>
+    <t>nov stdev</t>
+  </si>
+  <si>
+    <t>oct stdev</t>
   </si>
 </sst>
 </file>
@@ -946,10 +955,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG870"/>
+  <dimension ref="A1:BD870"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="98" workbookViewId="0">
-      <selection activeCell="AD1" sqref="AD1:AG16"/>
+    <sheetView tabSelected="1" topLeftCell="AM1" zoomScale="98" workbookViewId="0">
+      <selection activeCell="AX19" sqref="AX19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1611,6 +1620,9 @@
       <c r="AB12">
         <v>63.3</v>
       </c>
+      <c r="AD12" t="s">
+        <v>26</v>
+      </c>
       <c r="AF12" t="e">
         <f ca="1">mad(F:AB)</f>
         <v>#NAME?</v>
@@ -1668,6 +1680,10 @@
       <c r="AB13">
         <v>66.2</v>
       </c>
+      <c r="AD13">
+        <f>_xlfn.STDEV.S(AB:AB)</f>
+        <v>9.1108492943771004</v>
+      </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1834,8 +1850,11 @@
       <c r="AB16">
         <v>56.6</v>
       </c>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AD16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1887,8 +1906,12 @@
       <c r="AB17">
         <v>55.1</v>
       </c>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AD17">
+        <f>_xlfn.STDEV.S(Z:Z)</f>
+        <v>11.253768356259661</v>
+      </c>
+    </row>
+    <row r="18" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1940,8 +1963,11 @@
       <c r="AB18">
         <v>59.9</v>
       </c>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AZ18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1993,8 +2019,100 @@
       <c r="AB19">
         <v>59.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AH19">
+        <f>_xlfn.STDEV.S(F:F)</f>
+        <v>8.0012463442087771</v>
+      </c>
+      <c r="AI19" t="e">
+        <f t="shared" ref="AI19" si="0">_xlfn.STDEV.S(G:G)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ19">
+        <f t="shared" ref="AJ19:AY19" si="1">_xlfn.STDEV.S(H:H)</f>
+        <v>7.0521223979554604</v>
+      </c>
+      <c r="AK19" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AL19">
+        <f t="shared" si="1"/>
+        <v>6.2887925308674175</v>
+      </c>
+      <c r="AM19" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AN19">
+        <f t="shared" si="1"/>
+        <v>10.925090475270101</v>
+      </c>
+      <c r="AO19" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AP19">
+        <f t="shared" si="1"/>
+        <v>46.377342148047241</v>
+      </c>
+      <c r="AQ19" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AR19">
+        <f t="shared" si="1"/>
+        <v>86.21925986896909</v>
+      </c>
+      <c r="AS19" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AT19">
+        <f>_xlfn.STDEV.S(R:R)</f>
+        <v>61.3424369708288</v>
+      </c>
+      <c r="AU19" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AV19">
+        <f t="shared" si="1"/>
+        <v>31.904675783568873</v>
+      </c>
+      <c r="AW19" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AX19">
+        <f t="shared" si="1"/>
+        <v>20.857464759298246</v>
+      </c>
+      <c r="AY19" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AZ19">
+        <f>_xlfn.STDEV.S(X:X)</f>
+        <v>15.281153583340403</v>
+      </c>
+      <c r="BA19" t="e">
+        <f t="shared" ref="BA19:BD19" si="2">_xlfn.STDEV.S(Y:Y)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BB19">
+        <f t="shared" si="2"/>
+        <v>11.253768356259661</v>
+      </c>
+      <c r="BC19" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BD19">
+        <f t="shared" si="2"/>
+        <v>9.1108492943771004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2047,7 +2165,7 @@
         <v>62.9</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -2100,7 +2218,7 @@
         <v>62.2</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -2153,7 +2271,7 @@
         <v>59.5</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -2205,8 +2323,11 @@
       <c r="AB23">
         <v>59.7</v>
       </c>
-    </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AD23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -2258,8 +2379,12 @@
       <c r="AB24">
         <v>54</v>
       </c>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AD24">
+        <f>_xlfn.STDEV.S(AB:AB)</f>
+        <v>9.1108492943771004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -2312,7 +2437,7 @@
         <v>49.5</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -2365,7 +2490,7 @@
         <v>49.7</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -2418,7 +2543,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>19</v>
       </c>
@@ -2471,7 +2596,7 @@
         <v>49.5</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -2524,7 +2649,7 @@
         <v>57.1</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -2577,7 +2702,7 @@
         <v>61.5</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -2627,7 +2752,7 @@
         <v>64.599999999999994</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>19</v>
       </c>

</xml_diff>